<commit_message>
a whole bunch of documentation updates because I am a mad man
</commit_message>
<xml_diff>
--- a/hardware/JamiePartList.xlsx
+++ b/hardware/JamiePartList.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhian\source\Aaron-Robot\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B86415-1190-4578-8271-4F0202D807E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72C867-AEA5-453F-ADFC-ED5F823239E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{55B075A3-7C5D-48F4-BB65-04BCD371373F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{55B075A3-7C5D-48F4-BB65-04BCD371373F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical + Motors" sheetId="1" r:id="rId1"/>
     <sheet name="Electrical - Non Digikey" sheetId="2" r:id="rId2"/>
-    <sheet name="DigiKey PartList" sheetId="3" r:id="rId3"/>
+    <sheet name="DigiKey Robot PartList" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C4EDF8-2A31-4933-9153-280CEBF4CDAF}">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D24E7FE-C5FF-4CFE-B7C3-31F16000B7E6}">
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>